<commit_message>
add import excel barang
</commit_message>
<xml_diff>
--- a/public/excel/import-suplier.xlsx
+++ b/public/excel/import-suplier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\laragon\www\taremakmur\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3A85C0-D9F5-4DAD-AA15-2CE4CD8ACC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D447757-2B29-425B-A128-197A3A43323E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B24B9DA-2B2A-4680-B36E-EE7B8E5E991F}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,6 +441,9 @@
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">

</xml_diff>